<commit_message>
Change date to col 2 and desc to col 3 ~ Change text wrap of desc ~ Add time of completing challenge ~ Add header to xlsx file ~ Change test file accordingly ~ Add test xlsx file
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -2,40 +2,369 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="20850" windowHeight="12080" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="待完成点播" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="已完成点播" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
+  <fonts count="20">
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -43,15 +372,308 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -404,7 +1026,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -414,10 +1035,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -425,19 +1047,195 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>倾世</t>
+          <t>老板名称</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>伊甸百变怪路线，书包弯币d6，无限充能，
-禁令呑了
-每次拿道具前必须弯币，成功了拿其中一个，不管一个房间几个道具（一个房间两个道具，成功也只能拿一个，剩下3个道具继续roll，并不是2个道具，成功就可以拿2个），成功一次只能拿一个，另一个继续弯币，可以一直d6到想要的道具在弯币</t>
+          <t>点播时间</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2023-9-20 18:29</t>
+          <t>点播内容</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>老板</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2023-2-1 16:25</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>以撒真结局</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>我</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2023-2-1 16:55</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>以撒百变怪</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>你</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2023-6-7 22:55</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>里夏娃半心通关</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>老板</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2023-9-7 13:00</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>百变挑战
+百变怪道具+d无穷+百变怪结局</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>我</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2023-9-12 22:25</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>mod：Bestia，lil plumy，MgTexture
+道具：书包 启示录
+路线：回溯线，但前两层找大可爱（没找到spawn 908.0）走陵墓1找塞壬（没找到spawn 904.0.0）
+要求：尽量拍启示录出四天启
+到妈腿打完能进br就进，要打完（濒死允许传送出来）
+如果加次数可以多打结局就大霍恩结束前stage去打撒旦，大撒旦和百变（按顺序）
+（可选，多一个点播次数）鉴赏/锐评见到的娘化boss的特点，自己是否喜欢等
+打的时候@我一下</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>大老板</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2023-10-1 22:25</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>插播：里犹大无道具见证者</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>中老板</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2023-9-30 21:20</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>插播：东方mod哆来咪终点</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>小老板</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2023-9-29 14：00</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>东方mod打幻想曲</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>小老板</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2023-9-10 13：00</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>东方mod打幻想曲</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>小老板</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2023-9-22 15：00</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>东方mod打幻想曲</t>
         </is>
       </c>
     </row>
@@ -452,114 +1250,38 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
+  <cols>
+    <col width="17.7272727272727" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>感染者_煌</t>
+          <t>老板名称</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>插播：点播队列程序测试</t>
+          <t>点播时间</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2023-9-23 19:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>fhfd</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>蓝人，挑战34，tm训练家，加命菇(每次死亡后可以深情告白一次来获得一个加命菇)，虚空(只能且必须吸掉所有主动道具，PS：会导致无法进行游戏的除外)，debug8，拿取全部道具(会导致无法进行游戏的除外)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2023-9-20 13:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>fhfd</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>亚波伦，书包534，合成袋710，妈妈的手镯604，吞下石化大便2，每次遇到道具时生成一个1499：Giant Poop巨型大便，进入boss房前生成一个巨型大便，并使用妈妈的手镯扔向boss，只能拿取合成袋生成的道具和大便道具，只能使用大便掉落物合成道具，击败和大便有关的boss后生成一个巨型大便。</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2023-9-20 13:35</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>fhfd</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>表抹大拉，旧绷带219，高凝血724，瘸子225，玻璃碎片448，糖心671，魂心吊坠686，黑怀412，妈妈的高跟鞋30，白羊座300，蒙眼。</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2023-9-20 13:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>fhfd</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>伊甸，D100283，吞下应急按钮149，金禁令88，金破口袋158，金40475，debug8</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2023-9-20 13:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Cuerzor</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>东方MOD+bydMOD
-里腐烂， 初始道具Corrupt Heart</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2023-9-20 17:17</t>
+          <t>点播内容</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>完成时间</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Style the header and columns ~ Add handler for PermissionError caused by concurrent editing
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -618,10 +618,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1043,19 +1046,24 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="80" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="20" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>老板名称</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>点播时间</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>点播内容</t>
         </is>

</xml_diff>